<commit_message>
LIMS Reg, SM,Stability Management Updated
</commit_message>
<xml_diff>
--- a/LIMS User Details For Automation.xlsx
+++ b/LIMS User Details For Automation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="19410" windowHeight="6495" firstSheet="2" activeTab="2"/>
@@ -10,25 +10,26 @@
     <sheet name="OrgNode" sheetId="14" r:id="rId1"/>
     <sheet name="AdminDepartment" sheetId="15" r:id="rId2"/>
     <sheet name="UserCreation" sheetId="5" r:id="rId3"/>
-    <sheet name="SampleRole" sheetId="6" r:id="rId4"/>
-    <sheet name="StabilityRole" sheetId="7" r:id="rId5"/>
-    <sheet name="MCRole" sheetId="8" r:id="rId6"/>
-    <sheet name="CAPARole" sheetId="9" r:id="rId7"/>
-    <sheet name="INVRole" sheetId="10" r:id="rId8"/>
-    <sheet name="RARole" sheetId="11" r:id="rId9"/>
-    <sheet name="AMRole" sheetId="12" r:id="rId10"/>
-    <sheet name="INCRole" sheetId="13" r:id="rId11"/>
-    <sheet name="UserGroup" sheetId="16" r:id="rId12"/>
-    <sheet name="CheckList" sheetId="18" r:id="rId13"/>
-    <sheet name="Sheet2" sheetId="22" r:id="rId14"/>
-    <sheet name="Sheet1" sheetId="23" r:id="rId15"/>
+    <sheet name="RegistrationRole" sheetId="24" r:id="rId4"/>
+    <sheet name="SampleRole" sheetId="6" r:id="rId5"/>
+    <sheet name="StabilityRole" sheetId="7" r:id="rId6"/>
+    <sheet name="MCRole" sheetId="8" r:id="rId7"/>
+    <sheet name="CAPARole" sheetId="9" r:id="rId8"/>
+    <sheet name="INVRole" sheetId="10" r:id="rId9"/>
+    <sheet name="RARole" sheetId="11" r:id="rId10"/>
+    <sheet name="AMRole" sheetId="12" r:id="rId11"/>
+    <sheet name="INCRole" sheetId="13" r:id="rId12"/>
+    <sheet name="UserGroup" sheetId="16" r:id="rId13"/>
+    <sheet name="CheckList" sheetId="18" r:id="rId14"/>
+    <sheet name="Sheet2" sheetId="22" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="23" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="199">
   <si>
     <t>Location</t>
   </si>
@@ -595,13 +596,43 @@
   </si>
   <si>
     <t>STLastName</t>
+  </si>
+  <si>
+    <t>Registration_FirstName</t>
+  </si>
+  <si>
+    <t>Registration_LastName</t>
+  </si>
+  <si>
+    <t>REGAUTO1</t>
+  </si>
+  <si>
+    <t>REGAUTO2</t>
+  </si>
+  <si>
+    <t>REGAUTO</t>
+  </si>
+  <si>
+    <t>REG001</t>
+  </si>
+  <si>
+    <t>REG002</t>
+  </si>
+  <si>
+    <t>Plant-1</t>
+  </si>
+  <si>
+    <t>Plant-1-QC</t>
+  </si>
+  <si>
+    <t>Plant-1-QA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -677,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -685,6 +716,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,6 +726,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -742,7 +777,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -774,9 +809,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -808,6 +844,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -983,21 +1020,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -1008,7 +1045,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -1019,7 +1056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -1030,7 +1067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -1047,19 +1084,109 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1067,7 +1194,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
@@ -1075,7 +1202,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
@@ -1083,7 +1210,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
@@ -1091,7 +1218,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>69</v>
       </c>
@@ -1099,7 +1226,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>70</v>
       </c>
@@ -1107,7 +1234,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
@@ -1115,7 +1242,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -1123,7 +1250,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
@@ -1131,7 +1258,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
@@ -1139,7 +1266,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>75</v>
       </c>
@@ -1147,7 +1274,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>76</v>
       </c>
@@ -1155,7 +1282,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>77</v>
       </c>
@@ -1163,7 +1290,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>78</v>
       </c>
@@ -1171,7 +1298,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>79</v>
       </c>
@@ -1184,20 +1311,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="A18:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1205,7 +1332,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1213,7 +1340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1221,7 +1348,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -1229,7 +1356,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -1237,7 +1364,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -1245,7 +1372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
@@ -1253,7 +1380,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>39</v>
       </c>
@@ -1261,7 +1388,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -1269,7 +1396,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1277,7 +1404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -1285,7 +1412,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -1293,7 +1420,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -1301,7 +1428,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
@@ -1309,7 +1436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -1317,7 +1444,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -1325,7 +1452,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1338,15 +1465,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1354,7 +1481,7 @@
     <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -1368,7 +1495,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1382,7 +1509,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1396,7 +1523,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1410,7 +1537,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -1429,21 +1556,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -1451,7 +1578,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -1459,7 +1586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -1472,21 +1599,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -1506,7 +1633,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -1526,7 +1653,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
@@ -1546,7 +1673,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
@@ -1566,7 +1693,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>128</v>
       </c>
@@ -1586,7 +1713,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>131</v>
       </c>
@@ -1606,7 +1733,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>134</v>
       </c>
@@ -1626,7 +1753,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>137</v>
       </c>
@@ -1646,7 +1773,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>140</v>
       </c>
@@ -1666,7 +1793,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>142</v>
       </c>
@@ -1686,7 +1813,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>144</v>
       </c>
@@ -1706,7 +1833,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>146</v>
       </c>
@@ -1726,7 +1853,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>148</v>
       </c>
@@ -1746,7 +1873,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>150</v>
       </c>
@@ -1766,7 +1893,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>152</v>
       </c>
@@ -1786,7 +1913,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>154</v>
       </c>
@@ -1806,7 +1933,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>157</v>
       </c>
@@ -1826,7 +1953,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>159</v>
       </c>
@@ -1846,7 +1973,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>161</v>
       </c>
@@ -1866,7 +1993,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>163</v>
       </c>
@@ -1886,7 +2013,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>165</v>
       </c>
@@ -1906,7 +2033,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>167</v>
       </c>
@@ -1926,7 +2053,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>169</v>
       </c>
@@ -1946,7 +2073,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>171</v>
       </c>
@@ -1966,7 +2093,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -1986,7 +2113,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>175</v>
       </c>
@@ -2006,7 +2133,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>177</v>
       </c>
@@ -2026,7 +2153,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>179</v>
       </c>
@@ -2046,7 +2173,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>181</v>
       </c>
@@ -2071,17 +2198,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>184</v>
       </c>
@@ -2092,7 +2219,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>119</v>
       </c>
@@ -2103,7 +2230,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>119</v>
       </c>
@@ -2114,7 +2241,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>119</v>
       </c>
@@ -2125,7 +2252,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>119</v>
       </c>
@@ -2136,7 +2263,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>119</v>
       </c>
@@ -2147,7 +2274,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>119</v>
       </c>
@@ -2158,7 +2285,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>119</v>
       </c>
@@ -2169,7 +2296,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>119</v>
       </c>
@@ -2180,7 +2307,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>119</v>
       </c>
@@ -2191,7 +2318,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>119</v>
       </c>
@@ -2202,7 +2329,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>119</v>
       </c>
@@ -2213,7 +2340,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>119</v>
       </c>
@@ -2224,7 +2351,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>119</v>
       </c>
@@ -2235,7 +2362,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>119</v>
       </c>
@@ -2252,20 +2379,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -2276,7 +2403,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2287,7 +2414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2298,7 +2425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2315,25 +2442,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -2353,565 +2477,133 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>191</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>119</v>
+        <v>193</v>
       </c>
       <c r="D6" s="1">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>133</v>
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>134</v>
+        <v>192</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>119</v>
+        <v>193</v>
       </c>
       <c r="D7" s="1">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>136</v>
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="1">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="1">
-        <v>11</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="1">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="1">
-        <v>13</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="1">
-        <v>14</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="1">
-        <v>15</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="1">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" s="1">
-        <v>17</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D18" s="1">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D19" s="1">
-        <v>4</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D20" s="1">
-        <v>5</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D21" s="1">
-        <v>6</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="1">
-        <v>7</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="1">
-        <v>11</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D24" s="1">
-        <v>12</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="1">
-        <v>13</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" s="1">
-        <v>14</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D27" s="1">
-        <v>15</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="1">
-        <v>16</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D29" s="1">
-        <v>17</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2919,181 +2611,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="26" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>193</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="1">
-        <v>11</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10" s="1">
-        <v>12</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="1">
-        <v>13</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B12" s="1">
-        <v>14</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="1">
-        <v>15</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B14" s="1">
-        <v>16</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" s="1">
-        <v>17</v>
-      </c>
-      <c r="C15" s="5" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3103,21 +2663,106 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>187</v>
       </c>
@@ -3128,7 +2773,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>155</v>
       </c>
@@ -3139,7 +2784,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>155</v>
       </c>
@@ -3150,7 +2795,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>155</v>
       </c>
@@ -3158,127 +2803,6 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B9" s="1">
-        <v>11</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="1">
-        <v>12</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" s="1">
-        <v>13</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" s="1">
-        <v>14</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" s="1">
-        <v>15</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" s="1">
-        <v>16</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15" s="1">
-        <v>17</v>
-      </c>
-      <c r="C15" s="5" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3287,20 +2811,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -3308,7 +2832,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
@@ -3316,7 +2840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>57</v>
       </c>
@@ -3324,7 +2848,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -3332,7 +2856,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>59</v>
       </c>
@@ -3340,7 +2864,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>60</v>
       </c>
@@ -3348,7 +2872,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>61</v>
       </c>
@@ -3356,7 +2880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>62</v>
       </c>
@@ -3364,7 +2888,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>63</v>
       </c>
@@ -3372,7 +2896,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>64</v>
       </c>
@@ -3380,7 +2904,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>65</v>
       </c>
@@ -3393,21 +2917,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -3415,7 +2939,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -3423,7 +2947,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -3431,7 +2955,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -3439,7 +2963,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -3447,7 +2971,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -3455,7 +2979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -3463,7 +2987,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3471,7 +2995,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -3479,7 +3003,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -3487,7 +3011,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -3500,20 +3024,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -3521,7 +3045,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -3529,7 +3053,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -3537,7 +3061,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -3545,7 +3069,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -3553,7 +3077,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -3561,7 +3085,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -3569,7 +3093,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -3577,7 +3101,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -3585,7 +3109,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -3593,7 +3117,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -3601,7 +3125,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -3609,7 +3133,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -3617,7 +3141,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -3625,7 +3149,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -3633,7 +3157,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -3641,7 +3165,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
@@ -3649,7 +3173,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -3657,7 +3181,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -3665,7 +3189,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -3673,7 +3197,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -3681,7 +3205,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
@@ -3689,7 +3213,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>41</v>
       </c>
@@ -3697,7 +3221,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>43</v>
       </c>
@@ -3705,102 +3229,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sample Management Finished Product Code Update 	On 01052023
</commit_message>
<xml_diff>
--- a/LIMS User Details For Automation.xlsx
+++ b/LIMS User Details For Automation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="16"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="OrgNode" sheetId="14" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="216">
   <si>
     <t>Location</t>
   </si>
@@ -620,15 +620,6 @@
     <t>REG002</t>
   </si>
   <si>
-    <t>Plant-1</t>
-  </si>
-  <si>
-    <t>Plant-1-QC</t>
-  </si>
-  <si>
-    <t>Plant-1-QA</t>
-  </si>
-  <si>
     <t>Qualitative Test -1</t>
   </si>
   <si>
@@ -675,13 +666,25 @@
   </si>
   <si>
     <t>TestName</t>
+  </si>
+  <si>
+    <t>Plant-3</t>
+  </si>
+  <si>
+    <t>Plant-3-QC</t>
+  </si>
+  <si>
+    <t>Plant-3-PF</t>
+  </si>
+  <si>
+    <t>Plant-3-QA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -832,7 +835,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -864,9 +867,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -898,6 +902,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1073,21 +1078,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -1098,7 +1103,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -1109,7 +1114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -1120,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -1137,19 +1142,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1157,7 +1162,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -1165,7 +1170,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
@@ -1173,7 +1178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -1181,7 +1186,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -1189,7 +1194,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
@@ -1197,7 +1202,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -1205,7 +1210,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
@@ -1213,7 +1218,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1227,19 +1232,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1247,7 +1252,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
@@ -1255,7 +1260,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
@@ -1263,7 +1268,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
@@ -1271,7 +1276,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>69</v>
       </c>
@@ -1279,7 +1284,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>70</v>
       </c>
@@ -1287,7 +1292,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
@@ -1295,7 +1300,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -1303,7 +1308,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
@@ -1311,7 +1316,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
@@ -1319,7 +1324,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>75</v>
       </c>
@@ -1327,7 +1332,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>76</v>
       </c>
@@ -1335,7 +1340,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>77</v>
       </c>
@@ -1343,7 +1348,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>78</v>
       </c>
@@ -1351,7 +1356,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>79</v>
       </c>
@@ -1365,19 +1370,19 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="A18:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1385,7 +1390,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1393,7 +1398,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1401,7 +1406,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -1409,7 +1414,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -1417,7 +1422,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -1425,7 +1430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
@@ -1433,7 +1438,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>39</v>
       </c>
@@ -1441,7 +1446,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -1449,7 +1454,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1457,7 +1462,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -1465,7 +1470,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -1473,7 +1478,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -1481,7 +1486,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
@@ -1489,7 +1494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -1497,7 +1502,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -1505,7 +1510,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1519,22 +1524,22 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="40.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -1548,7 +1553,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1562,7 +1567,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1576,7 +1581,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1590,7 +1595,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -1610,20 +1615,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -1631,7 +1636,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -1639,7 +1644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -1653,20 +1658,20 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -1686,7 +1691,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -1706,7 +1711,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
@@ -1726,7 +1731,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
@@ -1746,7 +1751,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>128</v>
       </c>
@@ -1766,7 +1771,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>131</v>
       </c>
@@ -1786,7 +1791,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>134</v>
       </c>
@@ -1806,7 +1811,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>137</v>
       </c>
@@ -1826,7 +1831,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>140</v>
       </c>
@@ -1846,7 +1851,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>142</v>
       </c>
@@ -1866,7 +1871,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>144</v>
       </c>
@@ -1886,7 +1891,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>146</v>
       </c>
@@ -1906,7 +1911,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>148</v>
       </c>
@@ -1926,7 +1931,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>150</v>
       </c>
@@ -1946,7 +1951,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>152</v>
       </c>
@@ -1966,7 +1971,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>154</v>
       </c>
@@ -1986,7 +1991,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>157</v>
       </c>
@@ -2006,7 +2011,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>159</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>161</v>
       </c>
@@ -2046,7 +2051,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>163</v>
       </c>
@@ -2066,7 +2071,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>165</v>
       </c>
@@ -2086,7 +2091,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>167</v>
       </c>
@@ -2106,7 +2111,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>169</v>
       </c>
@@ -2126,7 +2131,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>171</v>
       </c>
@@ -2146,7 +2151,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>173</v>
       </c>
@@ -2166,7 +2171,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>175</v>
       </c>
@@ -2186,7 +2191,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>177</v>
       </c>
@@ -2206,7 +2211,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>179</v>
       </c>
@@ -2226,7 +2231,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>181</v>
       </c>
@@ -2252,16 +2257,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>184</v>
       </c>
@@ -2272,7 +2277,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>119</v>
       </c>
@@ -2283,7 +2288,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>119</v>
       </c>
@@ -2294,7 +2299,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>119</v>
       </c>
@@ -2305,7 +2310,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>119</v>
       </c>
@@ -2316,7 +2321,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>119</v>
       </c>
@@ -2327,7 +2332,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>119</v>
       </c>
@@ -2338,7 +2343,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>119</v>
       </c>
@@ -2349,7 +2354,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>119</v>
       </c>
@@ -2360,7 +2365,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>119</v>
       </c>
@@ -2371,7 +2376,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>119</v>
       </c>
@@ -2382,7 +2387,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>119</v>
       </c>
@@ -2393,7 +2398,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>119</v>
       </c>
@@ -2404,7 +2409,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>119</v>
       </c>
@@ -2415,7 +2420,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>119</v>
       </c>
@@ -2432,121 +2437,121 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B10" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="B11" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="B12" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>204</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2556,20 +2561,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -2580,7 +2585,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2591,7 +2596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2602,7 +2607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2619,22 +2624,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -2654,12 +2659,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>119</v>
@@ -2671,15 +2676,15 @@
         <v>120</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>119</v>
@@ -2691,15 +2696,15 @@
         <v>124</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>193</v>
@@ -2711,15 +2716,15 @@
         <v>194</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>193</v>
@@ -2731,15 +2736,15 @@
         <v>195</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>154</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>155</v>
@@ -2751,15 +2756,15 @@
         <v>156</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>155</v>
@@ -2771,15 +2776,15 @@
         <v>158</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>155</v>
@@ -2791,15 +2796,15 @@
         <v>160</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>119</v>
@@ -2811,7 +2816,7 @@
         <v>127</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2820,20 +2825,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="26" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>189</v>
       </c>
@@ -2844,7 +2849,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>193</v>
       </c>
@@ -2855,7 +2860,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>193</v>
       </c>
@@ -2872,20 +2877,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="26" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>184</v>
       </c>
@@ -2896,7 +2901,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
@@ -2907,7 +2912,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>119</v>
       </c>
@@ -2918,7 +2923,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>119</v>
       </c>
@@ -2929,7 +2934,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>193</v>
       </c>
@@ -2940,7 +2945,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>193</v>
       </c>
@@ -2957,21 +2962,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>187</v>
       </c>
@@ -2982,7 +2987,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>155</v>
       </c>
@@ -2993,7 +2998,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>155</v>
       </c>
@@ -3004,7 +3009,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>155</v>
       </c>
@@ -3021,19 +3026,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -3041,7 +3046,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
@@ -3049,7 +3054,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>57</v>
       </c>
@@ -3057,7 +3062,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -3065,7 +3070,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>59</v>
       </c>
@@ -3073,7 +3078,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>60</v>
       </c>
@@ -3081,7 +3086,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>61</v>
       </c>
@@ -3089,7 +3094,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>62</v>
       </c>
@@ -3097,7 +3102,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>63</v>
       </c>
@@ -3105,7 +3110,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>64</v>
       </c>
@@ -3113,7 +3118,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>65</v>
       </c>
@@ -3127,20 +3132,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -3148,7 +3153,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -3156,7 +3161,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -3164,7 +3169,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -3172,7 +3177,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -3180,7 +3185,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -3188,7 +3193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -3196,7 +3201,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3204,7 +3209,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -3212,7 +3217,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -3220,7 +3225,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -3234,19 +3239,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -3254,7 +3259,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -3262,7 +3267,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -3270,7 +3275,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -3278,7 +3283,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -3286,7 +3291,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -3294,7 +3299,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -3302,7 +3307,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -3310,7 +3315,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -3318,7 +3323,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -3326,7 +3331,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -3334,7 +3339,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -3342,7 +3347,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -3350,7 +3355,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -3358,7 +3363,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -3366,7 +3371,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -3374,7 +3379,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
@@ -3382,7 +3387,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -3390,7 +3395,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -3398,7 +3403,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -3406,7 +3411,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -3414,7 +3419,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
@@ -3422,7 +3427,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>41</v>
       </c>
@@ -3430,7 +3435,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>43</v>
       </c>
@@ -3438,7 +3443,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Lims Update from Lakshman System
</commit_message>
<xml_diff>
--- a/LIMS User Details For Automation.xlsx
+++ b/LIMS User Details For Automation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="11" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="OrgNode" sheetId="14" r:id="rId1"/>
@@ -13,24 +13,26 @@
     <sheet name="RegistrationRole" sheetId="24" r:id="rId4"/>
     <sheet name="SampleRole" sheetId="6" r:id="rId5"/>
     <sheet name="StabilityRole" sheetId="7" r:id="rId6"/>
-    <sheet name="MCRole" sheetId="8" r:id="rId7"/>
-    <sheet name="CAPARole" sheetId="9" r:id="rId8"/>
-    <sheet name="INVRole" sheetId="10" r:id="rId9"/>
-    <sheet name="RARole" sheetId="11" r:id="rId10"/>
-    <sheet name="AMRole" sheetId="12" r:id="rId11"/>
-    <sheet name="INCRole" sheetId="13" r:id="rId12"/>
-    <sheet name="UserGroup" sheetId="16" r:id="rId13"/>
-    <sheet name="CheckList" sheetId="18" r:id="rId14"/>
-    <sheet name="Sheet2" sheetId="22" r:id="rId15"/>
-    <sheet name="Sheet1" sheetId="23" r:id="rId16"/>
-    <sheet name="TestDetails" sheetId="25" r:id="rId17"/>
+    <sheet name="Sheet3" sheetId="26" r:id="rId7"/>
+    <sheet name="MCRole" sheetId="8" r:id="rId8"/>
+    <sheet name="CAPARole" sheetId="9" r:id="rId9"/>
+    <sheet name="INVRole" sheetId="10" r:id="rId10"/>
+    <sheet name="RARole" sheetId="11" r:id="rId11"/>
+    <sheet name="AMRole" sheetId="12" r:id="rId12"/>
+    <sheet name="INCRole" sheetId="13" r:id="rId13"/>
+    <sheet name="UserGroup" sheetId="16" r:id="rId14"/>
+    <sheet name="CheckList" sheetId="18" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="22" r:id="rId16"/>
+    <sheet name="Sheet1" sheetId="23" r:id="rId17"/>
+    <sheet name="TestDetails" sheetId="25" r:id="rId18"/>
+    <sheet name="RMTestDetails" sheetId="27" r:id="rId19"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="228">
   <si>
     <t>Location</t>
   </si>
@@ -668,16 +670,52 @@
     <t>TestName</t>
   </si>
   <si>
-    <t>Plant-3</t>
-  </si>
-  <si>
-    <t>Plant-3-QC</t>
-  </si>
-  <si>
-    <t>Plant-3-PF</t>
-  </si>
-  <si>
-    <t>Plant-3-QA</t>
+    <t>Plant-2-QC</t>
+  </si>
+  <si>
+    <t>Plant-2-PF</t>
+  </si>
+  <si>
+    <t>Plant-2-QA</t>
+  </si>
+  <si>
+    <t>Plant-2</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -2</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -1</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -3</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -4</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -5</t>
+  </si>
+  <si>
+    <t>RM Qualitative Test -6</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-1</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-2</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-3</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-4</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-5</t>
+  </si>
+  <si>
+    <t>RM Quantitative Test-6</t>
   </si>
 </sst>
 </file>
@@ -1143,6 +1181,224 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1231,7 +1487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -1369,7 +1625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -1523,7 +1779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1614,7 +1870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1657,7 +1913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
@@ -2256,7 +2512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -2436,12 +2692,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,6 +2813,129 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2628,7 +3007,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,7 +3043,7 @@
         <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>119</v>
@@ -2676,7 +3055,7 @@
         <v>120</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2684,7 +3063,7 @@
         <v>122</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>119</v>
@@ -2696,7 +3075,7 @@
         <v>124</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2704,7 +3083,7 @@
         <v>191</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>193</v>
@@ -2716,7 +3095,7 @@
         <v>194</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2724,7 +3103,7 @@
         <v>192</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>193</v>
@@ -2736,7 +3115,7 @@
         <v>195</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2744,7 +3123,7 @@
         <v>154</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>155</v>
@@ -2756,7 +3135,7 @@
         <v>156</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2764,7 +3143,7 @@
         <v>157</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>155</v>
@@ -2776,7 +3155,7 @@
         <v>158</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2784,7 +3163,7 @@
         <v>159</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>155</v>
@@ -2796,7 +3175,7 @@
         <v>160</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2804,7 +3183,7 @@
         <v>125</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>119</v>
@@ -2816,7 +3195,7 @@
         <v>127</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3027,6 +3406,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3131,7 +3522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -3236,222 +3627,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>